<commit_message>
updating infiltration literature chapter
</commit_message>
<xml_diff>
--- a/Figures/Figures.xlsx
+++ b/Figures/Figures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedroAlmeida\Documents\Thesis\Thesis-hydroinformatics\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD256A55-1363-4BEE-8E37-A303A8F6011D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{62EDBA9D-C3AA-4BE9-85B5-7CF803296ED2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11192,6 +11192,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000214AC3F95A27E41B3706ACC4666A717" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7e816977beac94ee907e91bab6f1ddc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b1747184-ff36-4a91-b447-e7412a8c5dd4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63f334e05ff93850ebaf241b590544e2" ns2:_="">
     <xsd:import namespace="b1747184-ff36-4a91-b447-e7412a8c5dd4"/>
@@ -11323,22 +11338,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F00A8BA2-3842-4696-8583-A0A0DCCD7192}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ECE611D-E8DA-4BB0-9CA0-9D630D7233EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b1747184-ff36-4a91-b447-e7412a8c5dd4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A68AAD8-AF43-466D-BED9-2AF62DE307A7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11354,28 +11378,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ECE611D-E8DA-4BB0-9CA0-9D630D7233EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b1747184-ff36-4a91-b447-e7412a8c5dd4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F00A8BA2-3842-4696-8583-A0A0DCCD7192}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>